<commit_message>
API subscribe error console
</commit_message>
<xml_diff>
--- a/src/assets/tamplate/l1schedule_upload_template.xlsx
+++ b/src/assets/tamplate/l1schedule_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pawan Kumar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A488568-C76C-42AF-9485-FD8A31A388B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECC0770-0E3F-4CE9-A771-7CD41AF9595D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>S No.</t>
   </si>
@@ -50,65 +50,84 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Website Development</t>
-  </si>
-  <si>
-    <t>Design wireframes for homepage</t>
-  </si>
-  <si>
-    <t>Develop HTML/CSS structure for the homepage</t>
-  </si>
-  <si>
-    <t>Implement JavaScript functionality for interactive elements</t>
-  </si>
-  <si>
-    <t>Marketing Campaign</t>
-  </si>
-  <si>
-    <t>Define target audience and segmentation criteria</t>
-  </si>
-  <si>
-    <t>Product Development</t>
-  </si>
-  <si>
-    <t>Conduct market research and competitive analysis</t>
-  </si>
-  <si>
-    <t>Define product requirements and features</t>
-  </si>
-  <si>
-    <t>Create wireframes and UI/UX design prototypes</t>
-  </si>
-  <si>
-    <t>Develop front-end components using React.js</t>
-  </si>
-  <si>
-    <t>Implement backend logic and database architecture</t>
-  </si>
-  <si>
-    <t>Integrate third-party APIs for additional functionality</t>
-  </si>
-  <si>
-    <t>Product Deployment</t>
+    <t>DSP MILESTONE / LOA</t>
+  </si>
+  <si>
+    <t>Date of LOA (SAIL DSP)</t>
+  </si>
+  <si>
+    <t>Agreement date/Vendor Registeration at DSP</t>
+  </si>
+  <si>
+    <t>Project Timeline</t>
+  </si>
+  <si>
+    <t>GEPDEC MILESTONE</t>
+  </si>
+  <si>
+    <t>Site Survey</t>
+  </si>
+  <si>
+    <t>Finalisation of contractor for Site</t>
+  </si>
+  <si>
+    <t>Mobilisation of Workpower - Civil Manpower</t>
+  </si>
+  <si>
+    <t>Completion of Design &amp; Engineering</t>
+  </si>
+  <si>
+    <t>Completion of Delivery of Supply Items</t>
+  </si>
+  <si>
+    <t>Completion of Civil activities.</t>
+  </si>
+  <si>
+    <t>Completon of Erection Activities</t>
+  </si>
+  <si>
+    <t>Testing &amp; Commissioning</t>
+  </si>
+  <si>
+    <t>ENGINEERING</t>
+  </si>
+  <si>
+    <t>Basic Engineering (Electrical and Civil)</t>
+  </si>
+  <si>
+    <t>Detail Engineering (Electrical)</t>
+  </si>
+  <si>
+    <t>Detail Engineering (Civil)</t>
+  </si>
+  <si>
+    <t>Equipment Engineering</t>
+  </si>
+  <si>
+    <t>Approval from CET</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>QTY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="Söhne"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -119,19 +138,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="Söhne"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -148,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,20 +167,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyFill="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyFill="0">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFill="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Date" xfId="3" xr:uid="{0DE99108-2818-4882-B213-A90EC8BF1357}"/>
+    <cellStyle name="Name" xfId="1" xr:uid="{48AFC514-8FE0-41D9-9A9C-552C64FC5F60}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Task" xfId="2" xr:uid="{DA32AE13-C844-416B-8F70-5095FABC8F9E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -501,227 +533,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
-        <v>45383</v>
-      </c>
-      <c r="D2" s="4">
-        <v>45386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="3">
+        <v>44615</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
-        <v>45383</v>
-      </c>
-      <c r="D3" s="4">
-        <v>45384</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="3">
+        <v>44615</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3</f>
+        <v>44615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.2</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
-        <v>45385</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45386</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
+      <c r="E4" s="3">
+        <v>44642</v>
+      </c>
+      <c r="F4" s="3">
+        <f>E4</f>
+        <v>44642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
-        <v>45386</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45386</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
+      <c r="E5" s="3">
+        <v>44642</v>
+      </c>
+      <c r="F5" s="3">
+        <f>E5+(18*30)</f>
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
-        <v>45387</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45388</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
+      <c r="E6" s="3">
+        <v>44463</v>
+      </c>
+      <c r="F6" s="3">
+        <v>45153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
-        <v>45386</v>
-      </c>
-      <c r="D7" s="4">
-        <v>45388</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
+      <c r="E7" s="3">
+        <v>44463</v>
+      </c>
+      <c r="F7" s="3">
+        <f>E7</f>
+        <v>44463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>44661</v>
+      </c>
+      <c r="F8" s="3">
+        <f>E8+20</f>
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3">
+        <f>F8+5</f>
+        <v>44686</v>
+      </c>
+      <c r="F9" s="3">
+        <f>E9+10</f>
+        <v>44696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3">
+        <v>44635</v>
+      </c>
+      <c r="F10" s="3">
+        <v>44864</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2.5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44681</v>
+      </c>
+      <c r="F11" s="3">
+        <v>45024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2.6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3">
+        <v>44696</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2.7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3">
+        <v>44875</v>
+      </c>
+      <c r="F13" s="3">
+        <v>45076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2.8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3">
+        <v>44986</v>
+      </c>
+      <c r="F14" s="3">
+        <v>45153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4">
-        <v>45389</v>
-      </c>
-      <c r="D8" s="4">
-        <v>45389</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75">
-      <c r="A9">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44635</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>3.1</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="4">
-        <v>45389</v>
-      </c>
-      <c r="D9" s="4">
-        <v>45389</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75">
-      <c r="A10">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3">
+        <v>44635</v>
+      </c>
+      <c r="F16" s="3">
+        <v>44694</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>3.2</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4">
-        <v>45390</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45390</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75">
-      <c r="A11">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3">
+        <v>44697</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>3.3</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4">
-        <v>45391</v>
-      </c>
-      <c r="D11" s="4">
-        <v>45391</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75">
-      <c r="A12">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3">
+        <v>44697</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44853</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>3.4</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4">
-        <v>45392</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45393</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75">
-      <c r="A13">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="3">
+        <v>44655</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44850</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>3.5</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4">
-        <v>45394</v>
-      </c>
-      <c r="D13" s="4">
-        <v>45394</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
-      <c r="A14">
-        <v>3.6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4">
-        <v>45395</v>
-      </c>
-      <c r="D14" s="4">
-        <v>45397</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="4">
-        <v>45398</v>
-      </c>
-      <c r="D15" s="4">
-        <v>45399</v>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3">
+        <f>E16+14</f>
+        <v>44649</v>
+      </c>
+      <c r="F20" s="3">
+        <f>F19+14</f>
+        <v>44864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>